<commit_message>
27 de junio actualizacion
</commit_message>
<xml_diff>
--- a/CONTROL_ALEXIS_ROMERO.xlsx
+++ b/CONTROL_ALEXIS_ROMERO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ARM\ControlGastos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186490C1-24BA-4720-8E90-EE138917A4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046F12BD-1193-4EA8-8A38-A2C03AA1FC5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="3" xr2:uid="{3FAFDB23-1CF5-4013-9B78-8B5AA99A5182}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="115">
   <si>
     <t>qty</t>
   </si>
@@ -305,43 +305,95 @@
     <t>CONTROL DE INGRESOS Y EGRESOS:</t>
   </si>
   <si>
-    <t>FECHA</t>
-  </si>
-  <si>
-    <t>INGRESO</t>
-  </si>
-  <si>
-    <t>EGRESO</t>
-  </si>
-  <si>
-    <t>CAPITAL INICIAL</t>
-  </si>
-  <si>
-    <t>TOTAL:</t>
-  </si>
-  <si>
-    <t>SALDO:</t>
-  </si>
-  <si>
-    <t>TOTAL INGRESO</t>
-  </si>
-  <si>
-    <t>TOTAL EGRESO</t>
-  </si>
-  <si>
-    <t>TOTALES</t>
+    <t>1 mesa chica + 6 sillas</t>
+  </si>
+  <si>
+    <t>1 mesa grande + 6 sillas</t>
+  </si>
+  <si>
+    <t>1 mesa grande + 8 sillas</t>
+  </si>
+  <si>
+    <t>COSTOS</t>
+  </si>
+  <si>
+    <t>1 hielera grande</t>
+  </si>
+  <si>
+    <t>DESGLOSE DE GANANCIAS DE ACUERDO A LOS PRECIOS:</t>
+  </si>
+  <si>
+    <t>VIERNES</t>
+  </si>
+  <si>
+    <t>SILLAS</t>
+  </si>
+  <si>
+    <t>MESAS CHICAS</t>
+  </si>
+  <si>
+    <t>MESAS GRANDES</t>
+  </si>
+  <si>
+    <t>HIELERAS GRANDES</t>
+  </si>
+  <si>
+    <t>BRINCA BRINCA 3x3</t>
+  </si>
+  <si>
+    <t>INVENTARIO INDIVIDUAL</t>
+  </si>
+  <si>
+    <t>INVENTARIO POR COMBOS</t>
+  </si>
+  <si>
+    <t>1 MESA CHICA + 4 SILLAS</t>
+  </si>
+  <si>
+    <t>8 JUEGOS</t>
+  </si>
+  <si>
+    <t>FALTAN SILLAS</t>
+  </si>
+  <si>
+    <t>SABADO</t>
+  </si>
+  <si>
+    <t>DOMINGO</t>
+  </si>
+  <si>
+    <t>8 COMBOS CHICOS</t>
+  </si>
+  <si>
+    <t>4 HIELERAS</t>
+  </si>
+  <si>
+    <t>4 HIELERAS (INDIVIDUALES)</t>
+  </si>
+  <si>
+    <t>combo 1 mesa chica + 4 sillas</t>
+  </si>
+  <si>
+    <t>4 brinca brincas</t>
+  </si>
+  <si>
+    <t>1 brinca brinca</t>
+  </si>
+  <si>
+    <t>1 MESA GRANDE + 6 sillas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -453,8 +505,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -531,8 +620,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FA00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -592,13 +699,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -662,6 +787,10 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -683,25 +812,48 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="21" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bueno" xfId="1" builtinId="26"/>
     <cellStyle name="Incorrecto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="11">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -812,18 +964,12 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FA00"/>
       <color rgb="FF28CD41"/>
-      <color rgb="FF00FA00"/>
     </mruColors>
   </colors>
   <extLst>
@@ -835,33 +981,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DBF203B9-D3EC-4D38-953D-15350ECE7D5C}" name="Tabla1" displayName="Tabla1" ref="A6:D8" totalsRowShown="0">
-  <autoFilter ref="A6:D8" xr:uid="{DBF203B9-D3EC-4D38-953D-15350ECE7D5C}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{489C5F4A-8927-46D7-BCBD-CDFABE9D1AB3}" name="FECHA"/>
-    <tableColumn id="2" xr3:uid="{CF70806B-E810-4A1C-BA9A-301F219AFE9D}" name="DESCRIPCION"/>
-    <tableColumn id="3" xr3:uid="{796B9485-1B10-449C-9ADB-0BD835C6D9D5}" name="INGRESO"/>
-    <tableColumn id="4" xr3:uid="{F81D1200-8249-4639-8642-7918AAFC84F0}" name="EGRESO"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8F50BF62-943F-44D4-BBE4-B76150A93187}" name="Tabla2" displayName="Tabla2" ref="B10:D12" totalsRowShown="0">
-  <autoFilter ref="B10:D12" xr:uid="{8F50BF62-943F-44D4-BBE4-B76150A93187}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{1C7C75B3-9954-490B-B2D9-C6E9F64941E3}" name="TOTALES" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{F05B19AA-6F7C-46AD-BBDF-42F8D6BF0ED7}" name="TOTAL INGRESO" dataDxfId="11">
-      <calculatedColumnFormula>C10-D10</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="3" xr3:uid="{866002AB-BFEE-4C84-AF1C-D69630F2AB41}" name="TOTAL EGRESO"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1702,17 +1821,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="24" t="s">
@@ -2116,10 +2235,10 @@
       <c r="I22" s="22"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="48" t="s">
+      <c r="A24" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="49"/>
+      <c r="B24" s="51"/>
       <c r="C24" s="30">
         <f>SUM(C5:C12)</f>
         <v>-3091.4974999999999</v>
@@ -2141,10 +2260,10 @@
       <c r="L24" s="21"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="50" t="s">
+      <c r="A25" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="50"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="32">
         <f>SUM(C3:C4)</f>
         <v>4499.68</v>
@@ -2166,10 +2285,10 @@
       <c r="L25" s="21"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="47" t="s">
+      <c r="A26" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="47"/>
+      <c r="B26" s="49"/>
       <c r="C26" s="29">
         <f>SUM(C3:C23)</f>
         <v>1408.1824999999999</v>
@@ -2349,21 +2468,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
       <c r="H1" s="41"/>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
       <c r="L1" s="41"/>
       <c r="M1" s="41"/>
     </row>
@@ -3454,112 +3573,290 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBE0ED7-8598-4BD1-88E7-F09E8A87B907}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.140625" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="58" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="57" t="s">
+      <c r="C1" s="59"/>
+      <c r="F1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="58" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="56" t="s">
+      <c r="C2" s="59"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="F3" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="G3" s="65" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="56"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="B4" s="54"/>
+      <c r="F4" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="67">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="F5" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="67">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75">
+      <c r="A6" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="57"/>
+      <c r="C6" s="57"/>
+      <c r="F6" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B7" s="56"/>
+      <c r="C7" s="55">
+        <v>80</v>
+      </c>
+      <c r="D7" s="45"/>
+      <c r="F7" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B8" s="56"/>
+      <c r="C8" s="55">
+        <v>100</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B9" s="56"/>
+      <c r="C9" s="55">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="56" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="52">
-        <v>45100</v>
-      </c>
-      <c r="B7" s="53" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="54">
-        <v>0</v>
-      </c>
-      <c r="D7" s="54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="C10" s="54" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="55">
+        <v>120</v>
+      </c>
+      <c r="D10" s="45"/>
+      <c r="F10" s="60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="56"/>
+      <c r="C11" s="55">
+        <v>250</v>
+      </c>
+      <c r="D11" s="45"/>
+      <c r="F11" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="56"/>
+      <c r="C12" s="55">
+        <v>350</v>
+      </c>
+      <c r="D12" s="45"/>
+      <c r="F12" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="56"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="55"/>
+      <c r="F13" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="G13" s="68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75">
+      <c r="B16" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="54" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="C11" s="54">
-        <f>SUM(C7:C8)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="54">
-        <f>SUM(D7:D8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="54">
-        <f>C11-D11</f>
-        <v>0</v>
+      <c r="C16" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="62" t="s">
+        <v>107</v>
+      </c>
+      <c r="E16" s="63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" s="55">
+        <f>8*$C$7</f>
+        <v>640</v>
+      </c>
+      <c r="C17" s="55">
+        <f t="shared" ref="C17:D17" si="0">8*$C$7</f>
+        <v>640</v>
+      </c>
+      <c r="D17" s="55">
+        <f t="shared" si="0"/>
+        <v>640</v>
+      </c>
+      <c r="E17" s="55">
+        <f>SUM(B17:D17)</f>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="64" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" s="55">
+        <f>4*$C$11</f>
+        <v>1000</v>
+      </c>
+      <c r="C18" s="55">
+        <f t="shared" ref="C18:D19" si="1">4*$C$11</f>
+        <v>1000</v>
+      </c>
+      <c r="D18" s="55">
+        <f t="shared" si="1"/>
+        <v>1000</v>
+      </c>
+      <c r="E18" s="55">
+        <f>SUM(B18:D18)</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="B19" s="55">
+        <f>4*$C$12</f>
+        <v>1400</v>
+      </c>
+      <c r="C19" s="55">
+        <f t="shared" ref="C19:E19" si="2">4*$C$12</f>
+        <v>1400</v>
+      </c>
+      <c r="D19" s="55">
+        <f t="shared" si="2"/>
+        <v>1400</v>
+      </c>
+      <c r="E19" s="55">
+        <f t="shared" si="2"/>
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75">
+      <c r="B21" s="61">
+        <f>SUM(B17:B19)</f>
+        <v>3040</v>
+      </c>
+      <c r="C21" s="61">
+        <f>SUM(C17:C19)</f>
+        <v>3040</v>
+      </c>
+      <c r="D21" s="61">
+        <f>SUM(D17:D19)</f>
+        <v>3040</v>
+      </c>
+      <c r="E21" s="61">
+        <f>SUM(E17:E19)</f>
+        <v>6320</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="11">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A6:C6"/>
   </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="2">
-    <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>